<commit_message>
update otw bab 5
</commit_message>
<xml_diff>
--- a/Bismillah Buku TA/Ujicoba.xlsx
+++ b/Bismillah Buku TA/Ujicoba.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\5112100100\Semester 8\Tugas Akhir\Bismillah Buku TA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\5112100100\Semester 8\Tugas Akhir\Program\tugasAkhir\Bismillah Buku TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="8280" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RBF sigma 1" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,24 +473,24 @@
       </c>
       <c r="B3" s="3">
         <f>(C3+D4)/(D4+D3+C3+C4)</f>
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C3" s="1">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2">
-        <v>4.6217000000000001E-2</v>
+        <v>3.7180999999999999E-2</v>
       </c>
       <c r="F3" s="3">
         <f>C3/(C3+D3)</f>
-        <v>0.75757575757575757</v>
+        <v>0.78260869565217395</v>
       </c>
       <c r="G3" s="3">
         <f>C3/(C3+C4)</f>
-        <v>0.78125</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -498,11 +498,11 @@
       <c r="B4" s="2"/>
       <c r="C4" s="1">
         <f>64-C3</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
         <f>56-D3</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -514,24 +514,24 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ref="B5" si="0">(C5+D6)/(D6+D5+C5+C6)</f>
-        <v>0.76666666666666672</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C5" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>5.0569000000000003E-2</v>
+        <v>3.4192E-2</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F12" si="1">C5/(C5+D5)</f>
-        <v>0.77272727272727271</v>
+        <f t="shared" ref="F5" si="1">C5/(C5+D5)</f>
+        <v>0.79104477611940294</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G12" si="2">C5/(C5+C6)</f>
-        <v>0.796875</v>
+        <f t="shared" ref="G5" si="2">C5/(C5+C6)</f>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -539,11 +539,11 @@
       <c r="B6" s="2"/>
       <c r="C6" s="1">
         <f>64-C5</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <f>56-D5</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -555,23 +555,23 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ref="B7" si="3">(C7+D8)/(D8+D7+C7+C8)</f>
-        <v>0.76666666666666672</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C7" s="1">
         <v>52</v>
       </c>
       <c r="D7" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2">
-        <v>3.7810999999999997E-2</v>
+        <v>3.4759999999999999E-2</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F12" si="4">C7/(C7+D7)</f>
-        <v>0.76470588235294112</v>
+        <f t="shared" ref="F7" si="4">C7/(C7+D7)</f>
+        <v>0.77611940298507465</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G12" si="5">C7/(C7+C8)</f>
+        <f t="shared" ref="G7" si="5">C7/(C7+C8)</f>
         <v>0.8125</v>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="D8" s="1">
         <f>56-D7</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -596,24 +596,24 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ref="B9" si="6">(C9+D10)/(D10+D9+C9+C10)</f>
-        <v>0.75</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C9" s="1">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2">
-        <v>5.2970999999999997E-2</v>
+        <v>3.4734000000000001E-2</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F12" si="7">C9/(C9+D9)</f>
-        <v>0.75757575757575757</v>
+        <f t="shared" ref="F9" si="7">C9/(C9+D9)</f>
+        <v>0.77611940298507465</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ref="G9:G12" si="8">C9/(C9+C10)</f>
-        <v>0.78125</v>
+        <f t="shared" ref="G9" si="8">C9/(C9+C10)</f>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -621,11 +621,11 @@
       <c r="B10" s="2"/>
       <c r="C10" s="1">
         <f>64-C9</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1">
         <f>56-D9</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -637,24 +637,24 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ref="B11" si="9">(C11+D12)/(D12+D11+C11+C12)</f>
-        <v>0.7583333333333333</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C11" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2">
-        <v>3.4599999999999999E-2</v>
+        <v>3.5031E-2</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ref="F11:F12" si="10">C11/(C11+D11)</f>
-        <v>0.76119402985074625</v>
+        <f t="shared" ref="F11" si="10">C11/(C11+D11)</f>
+        <v>0.77941176470588236</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ref="G11:G12" si="11">C11/(C11+C12)</f>
-        <v>0.796875</v>
+        <f t="shared" ref="G11" si="11">C11/(C11+C12)</f>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -662,11 +662,11 @@
       <c r="B12" s="2"/>
       <c r="C12" s="1">
         <f>64-C11</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1">
         <f>56-D11</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -676,21 +676,21 @@
       <c r="A13" s="2"/>
       <c r="B13" s="3">
         <f>AVERAGE(B3:B12)</f>
-        <v>0.7583333333333333</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2">
         <f>AVERAGE(E3:E12)</f>
-        <v>4.4433600000000004E-2</v>
+        <v>3.5179599999999998E-2</v>
       </c>
       <c r="F13" s="3">
         <f>AVERAGE(F3:F12)</f>
-        <v>0.76275574001649515</v>
+        <v>0.78106080848952175</v>
       </c>
       <c r="G13" s="3">
         <f>AVERAGE(G3:G12)</f>
-        <v>0.79374999999999996</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,24 +734,24 @@
       </c>
       <c r="B19" s="3">
         <f>(C19+D20)/(D20+D19+C19+C20)</f>
-        <v>0.78333333333333333</v>
+        <v>0.7583333333333333</v>
       </c>
       <c r="C19" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E19" s="2">
-        <v>8.9547000000000002E-2</v>
+        <v>7.9464999999999994E-2</v>
       </c>
       <c r="F19" s="3">
         <f>C19/(C19+D19)</f>
-        <v>0.76388888888888884</v>
+        <v>0.74647887323943662</v>
       </c>
       <c r="G19" s="3">
         <f>C19/(C19+C20)</f>
-        <v>0.859375</v>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -759,11 +759,11 @@
       <c r="B20" s="2"/>
       <c r="C20" s="1">
         <f>64-C19</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1">
         <f>56-D19</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -778,21 +778,21 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="C21" s="1">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2">
-        <v>8.1263000000000002E-2</v>
+        <v>7.7997999999999998E-2</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:F28" si="13">C21/(C21+D21)</f>
-        <v>0.78260869565217395</v>
+        <f t="shared" ref="F21" si="13">C21/(C21+D21)</f>
+        <v>0.76</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" ref="G21:G28" si="14">C21/(C21+C22)</f>
-        <v>0.84375</v>
+        <f t="shared" ref="G21" si="14">C21/(C21+C22)</f>
+        <v>0.890625</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -800,11 +800,11 @@
       <c r="B22" s="2"/>
       <c r="C22" s="1">
         <f>64-C21</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1">
         <f>56-D21</f>
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -816,24 +816,24 @@
       </c>
       <c r="B23" s="3">
         <f t="shared" ref="B23" si="15">(C23+D24)/(D24+D23+C23+C24)</f>
-        <v>0.7583333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="C23" s="1">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="2">
-        <v>8.0317E-2</v>
+        <v>0.118394</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ref="F23:F28" si="16">C23/(C23+D23)</f>
-        <v>0.74647887323943662</v>
+        <f t="shared" ref="F23" si="16">C23/(C23+D23)</f>
+        <v>0.77027027027027029</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ref="G23:G28" si="17">C23/(C23+C24)</f>
-        <v>0.828125</v>
+        <f t="shared" ref="G23" si="17">C23/(C23+C24)</f>
+        <v>0.890625</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -841,11 +841,11 @@
       <c r="B24" s="2"/>
       <c r="C24" s="1">
         <f>64-C23</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D24" s="1">
         <f>56-D23</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -857,24 +857,24 @@
       </c>
       <c r="B25" s="3">
         <f t="shared" ref="B25" si="18">(C25+D26)/(D26+D25+C25+C26)</f>
-        <v>0.77500000000000002</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C25" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="2">
-        <v>8.0979999999999996E-2</v>
+        <v>8.8523000000000004E-2</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" ref="F25:F28" si="19">C25/(C25+D25)</f>
-        <v>0.76811594202898548</v>
+        <f t="shared" ref="F25" si="19">C25/(C25+D25)</f>
+        <v>0.76388888888888884</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G28" si="20">C25/(C25+C26)</f>
-        <v>0.828125</v>
+        <f t="shared" ref="G25" si="20">C25/(C25+C26)</f>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -882,11 +882,11 @@
       <c r="B26" s="2"/>
       <c r="C26" s="1">
         <f>64-C25</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D26" s="1">
         <f>56-D25</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -898,24 +898,24 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" ref="B27" si="21">(C27+D28)/(D28+D27+C27+C28)</f>
-        <v>0.78333333333333333</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C27" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E27" s="2">
-        <v>8.3989999999999995E-2</v>
+        <v>7.8923999999999994E-2</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" ref="F27:F28" si="22">C27/(C27+D27)</f>
-        <v>0.77142857142857146</v>
+        <f t="shared" ref="F27" si="22">C27/(C27+D27)</f>
+        <v>0.75342465753424659</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" ref="G27:G28" si="23">C27/(C27+C28)</f>
-        <v>0.84375</v>
+        <f t="shared" ref="G27" si="23">C27/(C27+C28)</f>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -923,11 +923,11 @@
       <c r="B28" s="2"/>
       <c r="C28" s="1">
         <f>64-C27</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="1">
         <f>56-D27</f>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -937,21 +937,21 @@
       <c r="A29" s="2"/>
       <c r="B29" s="3">
         <f>AVERAGE(B19:B28)</f>
-        <v>0.77833333333333321</v>
+        <v>0.78166666666666651</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="2">
         <f>AVERAGE(E19:E28)</f>
-        <v>8.3219399999999999E-2</v>
+        <v>8.8660800000000012E-2</v>
       </c>
       <c r="F29" s="3">
         <f>AVERAGE(F19:F28)</f>
-        <v>0.76650419424761118</v>
+        <v>0.75881253798656845</v>
       </c>
       <c r="G29" s="3">
         <f>AVERAGE(G19:G28)</f>
-        <v>0.84062499999999996</v>
+        <v>0.86562499999999998</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,24 +995,24 @@
       </c>
       <c r="B35" s="3">
         <f>(C35+D36)/(D36+D35+C35+C36)</f>
-        <v>0.7583333333333333</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C35" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D35" s="1">
         <v>16</v>
       </c>
       <c r="E35" s="2">
-        <v>5.4671999999999998E-2</v>
+        <v>5.8471000000000002E-2</v>
       </c>
       <c r="F35" s="3">
         <f>C35/(C35+D35)</f>
-        <v>0.76119402985074625</v>
+        <v>0.76811594202898548</v>
       </c>
       <c r="G35" s="3">
         <f>C35/(C35+C36)</f>
-        <v>0.796875</v>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
       <c r="B36" s="2"/>
       <c r="C36" s="1">
         <f>64-C35</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D36" s="1">
         <f>56-D35</f>
@@ -1036,24 +1036,24 @@
       </c>
       <c r="B37" s="3">
         <f t="shared" ref="B37" si="24">(C37+D38)/(D38+D37+C37+C38)</f>
-        <v>0.76666666666666672</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C37" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="2">
-        <v>5.3460000000000001E-2</v>
+        <v>5.4016000000000002E-2</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:F44" si="25">C37/(C37+D37)</f>
-        <v>0.76470588235294112</v>
+        <f t="shared" ref="F37" si="25">C37/(C37+D37)</f>
+        <v>0.77941176470588236</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" ref="G37:G44" si="26">C37/(C37+C38)</f>
-        <v>0.8125</v>
+        <f t="shared" ref="G37" si="26">C37/(C37+C38)</f>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,11 +1061,11 @@
       <c r="B38" s="2"/>
       <c r="C38" s="1">
         <f>64-C37</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="1">
         <f>56-D37</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1077,24 +1077,24 @@
       </c>
       <c r="B39" s="3">
         <f t="shared" ref="B39" si="27">(C39+D40)/(D40+D39+C39+C40)</f>
-        <v>0.7583333333333333</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C39" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D39" s="1">
         <v>16</v>
       </c>
       <c r="E39" s="2">
-        <v>5.9651999999999997E-2</v>
+        <v>5.5947999999999998E-2</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ref="F39:F44" si="28">C39/(C39+D39)</f>
-        <v>0.76119402985074625</v>
+        <f t="shared" ref="F39" si="28">C39/(C39+D39)</f>
+        <v>0.76811594202898548</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" ref="G39:G44" si="29">C39/(C39+C40)</f>
-        <v>0.796875</v>
+        <f t="shared" ref="G39" si="29">C39/(C39+C40)</f>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
       <c r="B40" s="2"/>
       <c r="C40" s="1">
         <f>64-C39</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D40" s="1">
         <f>56-D39</f>
@@ -1118,24 +1118,24 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" ref="B41" si="30">(C41+D42)/(D42+D41+C41+C42)</f>
-        <v>0.75</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C41" s="1">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D41" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" s="2">
-        <v>5.4193999999999999E-2</v>
+        <v>5.4139E-2</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ref="F41:F44" si="31">C41/(C41+D41)</f>
-        <v>0.75757575757575757</v>
+        <f t="shared" ref="F41" si="31">C41/(C41+D41)</f>
+        <v>0.77941176470588236</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" ref="G41:G44" si="32">C41/(C41+C42)</f>
-        <v>0.78125</v>
+        <f t="shared" ref="G41" si="32">C41/(C41+C42)</f>
+        <v>0.828125</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1143,11 +1143,11 @@
       <c r="B42" s="2"/>
       <c r="C42" s="1">
         <f>64-C41</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D42" s="1">
         <f>56-D41</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1159,24 +1159,24 @@
       </c>
       <c r="B43" s="3">
         <f t="shared" ref="B43" si="33">(C43+D44)/(D44+D43+C43+C44)</f>
-        <v>0.75</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C43" s="1">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D43" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E43" s="2">
-        <v>5.2446E-2</v>
+        <v>5.3358999999999997E-2</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ref="F43:F44" si="34">C43/(C43+D43)</f>
-        <v>0.75757575757575757</v>
+        <f t="shared" ref="F43" si="34">C43/(C43+D43)</f>
+        <v>0.77611940298507465</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" ref="G43:G44" si="35">C43/(C43+C44)</f>
-        <v>0.78125</v>
+        <f t="shared" ref="G43" si="35">C43/(C43+C44)</f>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1184,11 +1184,11 @@
       <c r="B44" s="2"/>
       <c r="C44" s="1">
         <f>64-C43</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D44" s="1">
         <f>56-D43</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -1198,21 +1198,21 @@
       <c r="A45" s="2"/>
       <c r="B45" s="3">
         <f>AVERAGE(B35:B44)</f>
-        <v>0.7566666666666666</v>
+        <v>0.77833333333333332</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="2">
         <f>AVERAGE(E35:E44)</f>
-        <v>5.4884799999999997E-2</v>
+        <v>5.5186599999999995E-2</v>
       </c>
       <c r="F45" s="3">
         <f>AVERAGE(F35:F44)</f>
-        <v>0.76044909144118977</v>
+        <v>0.77423496329096209</v>
       </c>
       <c r="G45" s="3">
         <f>AVERAGE(G35:G44)</f>
-        <v>0.79374999999999996</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1226,67 +1226,31 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
@@ -1294,31 +1258,67 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1329,7 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -1371,24 +1371,24 @@
       </c>
       <c r="B3" s="3">
         <f>(C3+D4)/(D4+D3+C3+C4)</f>
-        <v>0.7583333333333333</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C3" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>3.6353000000000003E-2</v>
+        <v>4.0064000000000002E-2</v>
       </c>
       <c r="F3" s="3">
         <f>C3/(C3+D3)</f>
-        <v>0.81818181818181823</v>
+        <v>0.84210526315789469</v>
       </c>
       <c r="G3" s="3">
         <f>C3/(C3+C4)</f>
-        <v>0.703125</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1396,11 +1396,11 @@
       <c r="B4" s="2"/>
       <c r="C4" s="1">
         <f>64-C3</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <f>56-D3</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1412,24 +1412,24 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ref="B5" si="0">(C5+D6)/(D6+D5+C5+C6)</f>
-        <v>0.76666666666666672</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C5" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>4.5844000000000003E-2</v>
+        <v>3.5142E-2</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F12" si="1">C5/(C5+D5)</f>
-        <v>0.8214285714285714</v>
+        <f t="shared" ref="F5" si="1">C5/(C5+D5)</f>
+        <v>0.84210526315789469</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G12" si="2">C5/(C5+C6)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G5" si="2">C5/(C5+C6)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,11 +1437,11 @@
       <c r="B6" s="2"/>
       <c r="C6" s="1">
         <f>64-C5</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1">
         <f>56-D5</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1453,24 +1453,24 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ref="B7" si="3">(C7+D8)/(D8+D7+C7+C8)</f>
-        <v>0.76666666666666672</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C7" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>4.0565999999999998E-2</v>
+        <v>3.6379000000000002E-2</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F12" si="4">C7/(C7+D7)</f>
-        <v>0.8214285714285714</v>
+        <f t="shared" ref="F7" si="4">C7/(C7+D7)</f>
+        <v>0.8392857142857143</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G12" si="5">C7/(C7+C8)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G7" si="5">C7/(C7+C8)</f>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1478,11 +1478,11 @@
       <c r="B8" s="2"/>
       <c r="C8" s="1">
         <f>64-C7</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1">
         <f>56-D7</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1494,23 +1494,23 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ref="B9" si="6">(C9+D10)/(D10+D9+C9+C10)</f>
-        <v>0.7583333333333333</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C9" s="1">
         <v>45</v>
       </c>
       <c r="D9" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>4.4464999999999998E-2</v>
+        <v>3.4674999999999997E-2</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F12" si="7">C9/(C9+D9)</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" ref="F9" si="7">C9/(C9+D9)</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ref="G9:G12" si="8">C9/(C9+C10)</f>
+        <f t="shared" ref="G9" si="8">C9/(C9+C10)</f>
         <v>0.703125</v>
       </c>
     </row>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="D10" s="1">
         <f>56-D9</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1535,24 +1535,24 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ref="B11" si="9">(C11+D12)/(D12+D11+C11+C12)</f>
-        <v>0.76666666666666672</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C11" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1">
         <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>3.5793999999999999E-2</v>
+        <v>3.4959999999999998E-2</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ref="F11:F12" si="10">C11/(C11+D11)</f>
-        <v>0.8214285714285714</v>
+        <f t="shared" ref="F11" si="10">C11/(C11+D11)</f>
+        <v>0.82758620689655171</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ref="G11:G12" si="11">C11/(C11+C12)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G11" si="11">C11/(C11+C12)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
       <c r="B12" s="2"/>
       <c r="C12" s="1">
         <f>64-C11</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1">
         <f>56-D11</f>
@@ -1574,21 +1574,21 @@
       <c r="A13" s="2"/>
       <c r="B13" s="3">
         <f>AVERAGE(B3:B12)</f>
-        <v>0.76333333333333331</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2">
         <f>AVERAGE(E3:E12)</f>
-        <v>4.0604399999999999E-2</v>
+        <v>3.6243999999999998E-2</v>
       </c>
       <c r="F13" s="3">
         <f>AVERAGE(F3:F12)</f>
-        <v>0.82012987012987004</v>
+        <v>0.83688315616627784</v>
       </c>
       <c r="G13" s="3">
         <f>AVERAGE(G3:G12)</f>
-        <v>0.71250000000000002</v>
+        <v>0.73750000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,24 +1632,24 @@
       </c>
       <c r="B19" s="3">
         <f>(C19+D20)/(D20+D19+C19+C20)</f>
-        <v>0.77500000000000002</v>
+        <v>0.75</v>
       </c>
       <c r="C19" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1">
         <v>10</v>
       </c>
       <c r="E19" s="2">
-        <v>0.111355</v>
+        <v>9.9396999999999999E-2</v>
       </c>
       <c r="F19" s="3">
         <f>C19/(C19+D19)</f>
-        <v>0.82456140350877194</v>
+        <v>0.81481481481481477</v>
       </c>
       <c r="G19" s="3">
         <f>C19/(C19+C20)</f>
-        <v>0.734375</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1657,7 +1657,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="1">
         <f>64-C19</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1">
         <f>56-D19</f>
@@ -1673,24 +1673,24 @@
       </c>
       <c r="B21" s="3">
         <f t="shared" ref="B21" si="12">(C21+D22)/(D22+D21+C21+C22)</f>
-        <v>0.7583333333333333</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C21" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1">
         <v>10</v>
       </c>
       <c r="E21" s="2">
-        <v>0.115785</v>
+        <v>0.104737</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:F28" si="13">C21/(C21+D21)</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" ref="F21" si="13">C21/(C21+D21)</f>
+        <v>0.8214285714285714</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" ref="G21:G28" si="14">C21/(C21+C22)</f>
-        <v>0.703125</v>
+        <f t="shared" ref="G21" si="14">C21/(C21+C22)</f>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
       <c r="B22" s="2"/>
       <c r="C22" s="1">
         <f>64-C21</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1">
         <f>56-D21</f>
@@ -1714,24 +1714,24 @@
       </c>
       <c r="B23" s="3">
         <f t="shared" ref="B23" si="15">(C23+D24)/(D24+D23+C23+C24)</f>
-        <v>0.75</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C23" s="1">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D23" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2">
-        <v>0.11537799999999999</v>
+        <v>0.12781300000000001</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ref="F23:F28" si="16">C23/(C23+D23)</f>
-        <v>0.81481481481481477</v>
+        <f t="shared" ref="F23" si="16">C23/(C23+D23)</f>
+        <v>0.83636363636363631</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ref="G23:G28" si="17">C23/(C23+C24)</f>
-        <v>0.6875</v>
+        <f t="shared" ref="G23" si="17">C23/(C23+C24)</f>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1739,11 +1739,11 @@
       <c r="B24" s="2"/>
       <c r="C24" s="1">
         <f>64-C23</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1">
         <f>56-D23</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1755,24 +1755,24 @@
       </c>
       <c r="B25" s="3">
         <f t="shared" ref="B25" si="18">(C25+D26)/(D26+D25+C25+C26)</f>
-        <v>0.76666666666666672</v>
+        <v>0.7583333333333333</v>
       </c>
       <c r="C25" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="1">
         <v>10</v>
       </c>
       <c r="E25" s="2">
-        <v>0.101914</v>
+        <v>9.6762000000000001E-2</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" ref="F25:F28" si="19">C25/(C25+D25)</f>
-        <v>0.8214285714285714</v>
+        <f t="shared" ref="F25" si="19">C25/(C25+D25)</f>
+        <v>0.81818181818181823</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G28" si="20">C25/(C25+C26)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G25" si="20">C25/(C25+C26)</f>
+        <v>0.703125</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="1">
         <f>64-C25</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1">
         <f>56-D25</f>
@@ -1796,23 +1796,23 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" ref="B27" si="21">(C27+D28)/(D28+D27+C27+C28)</f>
-        <v>0.7583333333333333</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C27" s="1">
         <v>45</v>
       </c>
       <c r="D27" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="2">
-        <v>9.7768999999999995E-2</v>
+        <v>8.5637000000000005E-2</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" ref="F27:F28" si="22">C27/(C27+D27)</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" ref="F27" si="22">C27/(C27+D27)</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" ref="G27:G28" si="23">C27/(C27+C28)</f>
+        <f t="shared" ref="G27" si="23">C27/(C27+C28)</f>
         <v>0.703125</v>
       </c>
     </row>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="D28" s="1">
         <f>56-D27</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1835,21 +1835,21 @@
       <c r="A29" s="2"/>
       <c r="B29" s="3">
         <f>AVERAGE(B19:B28)</f>
-        <v>0.7616666666666666</v>
+        <v>0.76333333333333331</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="2">
         <f>AVERAGE(E19:E28)</f>
-        <v>0.10844019999999999</v>
+        <v>0.10286919999999999</v>
       </c>
       <c r="F29" s="3">
         <f>AVERAGE(F19:F28)</f>
-        <v>0.81943368522315896</v>
+        <v>0.8248244348244349</v>
       </c>
       <c r="G29" s="3">
         <f>AVERAGE(G19:G28)</f>
-        <v>0.70937499999999998</v>
+        <v>0.70625000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1893,24 +1893,24 @@
       </c>
       <c r="B35" s="3">
         <f>(C35+D36)/(D36+D35+C35+C36)</f>
-        <v>0.76666666666666672</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C35" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D35" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35" s="2">
-        <v>5.9228000000000003E-2</v>
+        <v>6.5386E-2</v>
       </c>
       <c r="F35" s="3">
         <f>C35/(C35+D35)</f>
-        <v>0.8214285714285714</v>
+        <v>0.8392857142857143</v>
       </c>
       <c r="G35" s="3">
         <f>C35/(C35+C36)</f>
-        <v>0.71875</v>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1918,11 +1918,11 @@
       <c r="B36" s="2"/>
       <c r="C36" s="1">
         <f>64-C35</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="1">
         <f>56-D35</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1934,24 +1934,24 @@
       </c>
       <c r="B37" s="3">
         <f t="shared" ref="B37" si="24">(C37+D38)/(D38+D37+C37+C38)</f>
-        <v>0.76666666666666672</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C37" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D37" s="1">
         <v>10</v>
       </c>
       <c r="E37" s="2">
-        <v>7.2911000000000004E-2</v>
+        <v>5.6689999999999997E-2</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:F44" si="25">C37/(C37+D37)</f>
-        <v>0.8214285714285714</v>
+        <f t="shared" ref="F37" si="25">C37/(C37+D37)</f>
+        <v>0.82758620689655171</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" ref="G37:G44" si="26">C37/(C37+C38)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G37" si="26">C37/(C37+C38)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1959,7 +1959,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="1">
         <f>64-C37</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D38" s="1">
         <f>56-D37</f>
@@ -1975,23 +1975,23 @@
       </c>
       <c r="B39" s="3">
         <f t="shared" ref="B39" si="27">(C39+D40)/(D40+D39+C39+C40)</f>
-        <v>0.7583333333333333</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C39" s="1">
         <v>45</v>
       </c>
       <c r="D39" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" s="2">
-        <v>6.3763E-2</v>
+        <v>5.8013000000000002E-2</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ref="F39:F44" si="28">C39/(C39+D39)</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" ref="F39" si="28">C39/(C39+D39)</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" ref="G39:G44" si="29">C39/(C39+C40)</f>
+        <f t="shared" ref="G39" si="29">C39/(C39+C40)</f>
         <v>0.703125</v>
       </c>
     </row>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="D40" s="1">
         <f>56-D39</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2016,24 +2016,24 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" ref="B41" si="30">(C41+D42)/(D42+D41+C41+C42)</f>
-        <v>0.7583333333333333</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C41" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D41" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" s="2">
-        <v>5.8741000000000002E-2</v>
+        <v>5.6561E-2</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ref="F41:F44" si="31">C41/(C41+D41)</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" ref="F41" si="31">C41/(C41+D41)</f>
+        <v>0.84210526315789469</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" ref="G41:G44" si="32">C41/(C41+C42)</f>
-        <v>0.703125</v>
+        <f t="shared" ref="G41" si="32">C41/(C41+C42)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2041,11 +2041,11 @@
       <c r="B42" s="2"/>
       <c r="C42" s="1">
         <f>64-C41</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D42" s="1">
         <f>56-D41</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -2057,24 +2057,24 @@
       </c>
       <c r="B43" s="3">
         <f t="shared" ref="B43" si="33">(C43+D44)/(D44+D43+C43+C44)</f>
-        <v>0.7583333333333333</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C43" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D43" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43" s="2">
-        <v>5.6112000000000002E-2</v>
+        <v>5.8636000000000001E-2</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ref="F43:F44" si="34">C43/(C43+D43)</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" ref="F43" si="34">C43/(C43+D43)</f>
+        <v>0.83636363636363631</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" ref="G43:G44" si="35">C43/(C43+C44)</f>
-        <v>0.703125</v>
+        <f t="shared" ref="G43" si="35">C43/(C43+C44)</f>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2082,11 +2082,11 @@
       <c r="B44" s="2"/>
       <c r="C44" s="1">
         <f>64-C43</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" s="1">
         <f>56-D43</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -2096,21 +2096,21 @@
       <c r="A45" s="2"/>
       <c r="B45" s="3">
         <f>AVERAGE(B35:B44)</f>
-        <v>0.76166666666666671</v>
+        <v>0.78</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="2">
         <f>AVERAGE(E35:E44)</f>
-        <v>6.2150999999999998E-2</v>
+        <v>5.9057199999999997E-2</v>
       </c>
       <c r="F45" s="3">
         <f>AVERAGE(F35:F44)</f>
-        <v>0.81948051948051948</v>
+        <v>0.83573483080742617</v>
       </c>
       <c r="G45" s="3">
         <f>AVERAGE(G35:G44)</f>
-        <v>0.70937499999999998</v>
+        <v>0.73124999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2124,67 +2124,31 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
@@ -2192,31 +2156,67 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2226,7 +2226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -2276,7 +2276,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>4.1095E-2</v>
+        <v>4.2341999999999998E-2</v>
       </c>
       <c r="F3" s="3">
         <f>C3/(C3+D3)</f>
@@ -2308,24 +2308,24 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ref="B5" si="0">(C5+D6)/(D6+D5+C5+C6)</f>
-        <v>0.78333333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="C5" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1">
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>4.0051999999999997E-2</v>
+        <v>3.5718E-2</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F12" si="1">C5/(C5+D5)</f>
-        <v>0.8392857142857143</v>
+        <f t="shared" ref="F5" si="1">C5/(C5+D5)</f>
+        <v>0.84482758620689657</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G12" si="2">C5/(C5+C6)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G5" si="2">C5/(C5+C6)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2333,7 +2333,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="1">
         <f>64-C5</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <f>56-D5</f>
@@ -2349,24 +2349,24 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ref="B7" si="3">(C7+D8)/(D8+D7+C7+C8)</f>
-        <v>0.7583333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="C7" s="1">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>3.8348E-2</v>
+        <v>3.7268999999999997E-2</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F12" si="4">C7/(C7+D7)</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" ref="F7" si="4">C7/(C7+D7)</f>
+        <v>0.84482758620689657</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G12" si="5">C7/(C7+C8)</f>
-        <v>0.703125</v>
+        <f t="shared" ref="G7" si="5">C7/(C7+C8)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2374,11 +2374,11 @@
       <c r="B8" s="2"/>
       <c r="C8" s="1">
         <f>64-C7</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
         <f>56-D7</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -2393,21 +2393,21 @@
         <v>0.78333333333333333</v>
       </c>
       <c r="C9" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>3.8973000000000001E-2</v>
+        <v>3.3161000000000003E-2</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F12" si="7">C9/(C9+D9)</f>
-        <v>0.8392857142857143</v>
+        <f t="shared" ref="F9" si="7">C9/(C9+D9)</f>
+        <v>0.82758620689655171</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ref="G9:G12" si="8">C9/(C9+C10)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G9" si="8">C9/(C9+C10)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2415,11 +2415,11 @@
       <c r="B10" s="2"/>
       <c r="C10" s="1">
         <f>64-C9</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
         <f>56-D9</f>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2431,24 +2431,24 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ref="B11" si="9">(C11+D12)/(D12+D11+C11+C12)</f>
-        <v>0.78333333333333333</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C11" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1">
         <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>3.3092999999999997E-2</v>
+        <v>3.4507999999999997E-2</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ref="F11:F12" si="10">C11/(C11+D11)</f>
-        <v>0.82758620689655171</v>
+        <f t="shared" ref="F11" si="10">C11/(C11+D11)</f>
+        <v>0.83050847457627119</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ref="G11:G12" si="11">C11/(C11+C12)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G11" si="11">C11/(C11+C12)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
       <c r="B12" s="2"/>
       <c r="C12" s="1">
         <f>64-C11</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1">
         <f>56-D11</f>
@@ -2470,21 +2470,21 @@
       <c r="A13" s="2"/>
       <c r="B13" s="3">
         <f>AVERAGE(B3:B12)</f>
-        <v>0.77833333333333332</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2">
         <f>AVERAGE(E3:E12)</f>
-        <v>3.8312199999999998E-2</v>
+        <v>3.6599599999999996E-2</v>
       </c>
       <c r="F13" s="3">
         <f>AVERAGE(F3:F12)</f>
-        <v>0.83038513210927012</v>
+        <v>0.83506721215663371</v>
       </c>
       <c r="G13" s="3">
         <f>AVERAGE(G3:G12)</f>
-        <v>0.734375</v>
+        <v>0.75937500000000002</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2528,24 +2528,24 @@
       </c>
       <c r="B19" s="3">
         <f>(C19+D20)/(D20+D19+C19+C20)</f>
-        <v>0.76666666666666672</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C19" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="2">
-        <v>7.6689999999999994E-2</v>
+        <v>7.6003000000000001E-2</v>
       </c>
       <c r="F19" s="3">
         <f>C19/(C19+D19)</f>
-        <v>0.81034482758620685</v>
+        <v>0.83050847457627119</v>
       </c>
       <c r="G19" s="3">
         <f>C19/(C19+C20)</f>
-        <v>0.734375</v>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2553,11 +2553,11 @@
       <c r="B20" s="2"/>
       <c r="C20" s="1">
         <f>64-C19</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1">
         <f>56-D19</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2569,24 +2569,24 @@
       </c>
       <c r="B21" s="3">
         <f t="shared" ref="B21" si="12">(C21+D22)/(D22+D21+C21+C22)</f>
-        <v>0.77500000000000002</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C21" s="1">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2">
-        <v>0.109734</v>
+        <v>8.0426999999999998E-2</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:F28" si="13">C21/(C21+D21)</f>
-        <v>0.81355932203389836</v>
+        <f t="shared" ref="F21" si="13">C21/(C21+D21)</f>
+        <v>0.80952380952380953</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" ref="G21:G28" si="14">C21/(C21+C22)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G21" si="14">C21/(C21+C22)</f>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2594,11 +2594,11 @@
       <c r="B22" s="2"/>
       <c r="C22" s="1">
         <f>64-C21</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1">
         <f>56-D21</f>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2610,24 +2610,24 @@
       </c>
       <c r="B23" s="3">
         <f t="shared" ref="B23" si="15">(C23+D24)/(D24+D23+C23+C24)</f>
-        <v>0.77500000000000002</v>
+        <v>0.80833333333333335</v>
       </c>
       <c r="C23" s="1">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="2">
-        <v>8.6865999999999999E-2</v>
+        <v>0.117171</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ref="F23:F28" si="16">C23/(C23+D23)</f>
-        <v>0.81355932203389836</v>
+        <f t="shared" ref="F23" si="16">C23/(C23+D23)</f>
+        <v>0.83606557377049184</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ref="G23:G28" si="17">C23/(C23+C24)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G23" si="17">C23/(C23+C24)</f>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2635,11 +2635,11 @@
       <c r="B24" s="2"/>
       <c r="C24" s="1">
         <f>64-C23</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1">
         <f>56-D23</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2651,24 +2651,24 @@
       </c>
       <c r="B25" s="3">
         <f t="shared" ref="B25" si="18">(C25+D26)/(D26+D25+C25+C26)</f>
-        <v>0.78333333333333333</v>
+        <v>0.81666666666666665</v>
       </c>
       <c r="C25" s="1">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D25" s="1">
         <v>9</v>
       </c>
       <c r="E25" s="2">
-        <v>9.5754000000000006E-2</v>
+        <v>9.5896999999999996E-2</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" ref="F25:F28" si="19">C25/(C25+D25)</f>
-        <v>0.8392857142857143</v>
+        <f t="shared" ref="F25" si="19">C25/(C25+D25)</f>
+        <v>0.85</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G28" si="20">C25/(C25+C26)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G25" si="20">C25/(C25+C26)</f>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2676,7 +2676,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="1">
         <f>64-C25</f>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D26" s="1">
         <f>56-D25</f>
@@ -2692,24 +2692,24 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" ref="B27" si="21">(C27+D28)/(D28+D27+C27+C28)</f>
-        <v>0.8</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C27" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="1">
         <v>11</v>
       </c>
       <c r="E27" s="2">
-        <v>7.6933000000000001E-2</v>
+        <v>7.9564999999999997E-2</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" ref="F27:F28" si="22">C27/(C27+D27)</f>
-        <v>0.82258064516129037</v>
+        <f t="shared" ref="F27" si="22">C27/(C27+D27)</f>
+        <v>0.81967213114754101</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" ref="G27:G28" si="23">C27/(C27+C28)</f>
-        <v>0.796875</v>
+        <f t="shared" ref="G27" si="23">C27/(C27+C28)</f>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
       <c r="B28" s="2"/>
       <c r="C28" s="1">
         <f>64-C27</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1">
         <f>56-D27</f>
@@ -2731,21 +2731,21 @@
       <c r="A29" s="2"/>
       <c r="B29" s="3">
         <f>AVERAGE(B19:B28)</f>
-        <v>0.78</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="2">
         <f>AVERAGE(E19:E28)</f>
-        <v>8.9195399999999994E-2</v>
+        <v>8.9812599999999992E-2</v>
       </c>
       <c r="F29" s="3">
         <f>AVERAGE(F19:F28)</f>
-        <v>0.81986596622020169</v>
+        <v>0.82915399780362264</v>
       </c>
       <c r="G29" s="3">
         <f>AVERAGE(G19:G28)</f>
-        <v>0.75312500000000004</v>
+        <v>0.78749999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2792,21 +2792,21 @@
         <v>0.8</v>
       </c>
       <c r="C35" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E35" s="2">
-        <v>0.255222</v>
+        <v>0.24393500000000001</v>
       </c>
       <c r="F35" s="3">
         <f>C35/(C35+D35)</f>
-        <v>0.84482758620689657</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G35" s="3">
         <f>C35/(C35+C36)</f>
-        <v>0.765625</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,11 +2814,11 @@
       <c r="B36" s="2"/>
       <c r="C36" s="1">
         <f>64-C35</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="1">
         <f>56-D35</f>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -2830,24 +2830,24 @@
       </c>
       <c r="B37" s="3">
         <f t="shared" ref="B37" si="24">(C37+D38)/(D38+D37+C37+C38)</f>
-        <v>0.77500000000000002</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C37" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D37" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" s="2">
-        <v>0.26950000000000002</v>
+        <v>0.239451</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:F44" si="25">C37/(C37+D37)</f>
-        <v>0.81355932203389836</v>
+        <f t="shared" ref="F37" si="25">C37/(C37+D37)</f>
+        <v>0.83050847457627119</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" ref="G37:G44" si="26">C37/(C37+C38)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G37" si="26">C37/(C37+C38)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2855,11 +2855,11 @@
       <c r="B38" s="2"/>
       <c r="C38" s="1">
         <f>64-C37</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="1">
         <f>56-D37</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -2880,14 +2880,14 @@
         <v>9</v>
       </c>
       <c r="E39" s="2">
-        <v>0.252029</v>
+        <v>0.275507</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ref="F39:F44" si="28">C39/(C39+D39)</f>
+        <f t="shared" ref="F39" si="28">C39/(C39+D39)</f>
         <v>0.84482758620689657</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" ref="G39:G44" si="29">C39/(C39+C40)</f>
+        <f t="shared" ref="G39" si="29">C39/(C39+C40)</f>
         <v>0.765625</v>
       </c>
     </row>
@@ -2921,14 +2921,14 @@
         <v>10</v>
       </c>
       <c r="E41" s="2">
-        <v>0.25184200000000001</v>
+        <v>0.23150599999999999</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ref="F41:F44" si="31">C41/(C41+D41)</f>
+        <f t="shared" ref="F41" si="31">C41/(C41+D41)</f>
         <v>0.82758620689655171</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" ref="G41:G44" si="32">C41/(C41+C42)</f>
+        <f t="shared" ref="G41" si="32">C41/(C41+C42)</f>
         <v>0.75</v>
       </c>
     </row>
@@ -2953,24 +2953,24 @@
       </c>
       <c r="B43" s="3">
         <f t="shared" ref="B43" si="33">(C43+D44)/(D44+D43+C43+C44)</f>
-        <v>0.77500000000000002</v>
+        <v>0.80833333333333335</v>
       </c>
       <c r="C43" s="1">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D43" s="1">
         <v>9</v>
       </c>
       <c r="E43" s="2">
-        <v>0.254691</v>
+        <v>0.23277300000000001</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ref="F43:F44" si="34">C43/(C43+D43)</f>
-        <v>0.83636363636363631</v>
+        <f t="shared" ref="F43" si="34">C43/(C43+D43)</f>
+        <v>0.84745762711864403</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" ref="G43:G44" si="35">C43/(C43+C44)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G43" si="35">C43/(C43+C44)</f>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2978,7 +2978,7 @@
       <c r="B44" s="2"/>
       <c r="C44" s="1">
         <f>64-C43</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D44" s="1">
         <f>56-D43</f>
@@ -2992,21 +2992,21 @@
       <c r="A45" s="2"/>
       <c r="B45" s="3">
         <f>AVERAGE(B35:B44)</f>
-        <v>0.78666666666666663</v>
+        <v>0.79666666666666663</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="2">
         <f>AVERAGE(E35:E44)</f>
-        <v>0.25665679999999996</v>
+        <v>0.24463439999999997</v>
       </c>
       <c r="F45" s="3">
         <f>AVERAGE(F35:F44)</f>
-        <v>0.83343286754157586</v>
+        <v>0.83674264562633949</v>
       </c>
       <c r="G45" s="3">
         <f>AVERAGE(G35:G44)</f>
-        <v>0.75</v>
+        <v>0.76875000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3020,67 +3020,31 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
@@ -3088,31 +3052,67 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3122,8 +3122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3163,24 +3163,24 @@
       </c>
       <c r="B3" s="3">
         <f>(C3+D4)/(D4+D3+C3+C4)</f>
-        <v>0.75</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C3" s="1">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1">
         <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>4.3143000000000001E-2</v>
+        <v>3.5410999999999998E-2</v>
       </c>
       <c r="F3" s="3">
         <f>C3/(C3+D3)</f>
-        <v>0.7931034482758621</v>
+        <v>0.80327868852459017</v>
       </c>
       <c r="G3" s="3">
         <f>C3/(C3+C4)</f>
-        <v>0.71875</v>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3188,7 +3188,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="1">
         <f>64-C3</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
         <f>56-D3</f>
@@ -3204,24 +3204,24 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ref="B5" si="0">(C5+D6)/(D6+D5+C5+C6)</f>
-        <v>0.77500000000000002</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C5" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
-        <v>3.8463999999999998E-2</v>
+        <v>3.4888000000000002E-2</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F12" si="1">C5/(C5+D5)</f>
-        <v>0.81355932203389836</v>
+        <f t="shared" ref="F5" si="1">C5/(C5+D5)</f>
+        <v>0.79032258064516125</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G12" si="2">C5/(C5+C6)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G5" si="2">C5/(C5+C6)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3229,11 +3229,11 @@
       <c r="B6" s="2"/>
       <c r="C6" s="1">
         <f>64-C5</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <f>56-D5</f>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -3245,24 +3245,24 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ref="B7" si="3">(C7+D8)/(D8+D7+C7+C8)</f>
-        <v>0.76666666666666672</v>
+        <v>0.7583333333333333</v>
       </c>
       <c r="C7" s="1">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2">
-        <v>3.4412999999999999E-2</v>
+        <v>3.6304000000000003E-2</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F12" si="4">C7/(C7+D7)</f>
-        <v>0.79032258064516125</v>
+        <f t="shared" ref="F7" si="4">C7/(C7+D7)</f>
+        <v>0.79661016949152541</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G12" si="5">C7/(C7+C8)</f>
-        <v>0.765625</v>
+        <f t="shared" ref="G7" si="5">C7/(C7+C8)</f>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3270,11 +3270,11 @@
       <c r="B8" s="2"/>
       <c r="C8" s="1">
         <f>64-C7</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1">
         <f>56-D7</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -3289,21 +3289,21 @@
         <v>0.7583333333333333</v>
       </c>
       <c r="C9" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2">
-        <v>3.7608000000000003E-2</v>
+        <v>3.3363999999999998E-2</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F12" si="7">C9/(C9+D9)</f>
-        <v>0.79661016949152541</v>
+        <f t="shared" ref="F9" si="7">C9/(C9+D9)</f>
+        <v>0.78688524590163933</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ref="G9:G12" si="8">C9/(C9+C10)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G9" si="8">C9/(C9+C10)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3311,11 +3311,11 @@
       <c r="B10" s="2"/>
       <c r="C10" s="1">
         <f>64-C9</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
         <f>56-D9</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -3327,24 +3327,24 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ref="B11" si="9">(C11+D12)/(D12+D11+C11+C12)</f>
-        <v>0.76666666666666672</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C11" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1">
         <v>12</v>
       </c>
       <c r="E11" s="2">
-        <v>3.8012999999999998E-2</v>
+        <v>3.1479E-2</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ref="F11:F12" si="10">C11/(C11+D11)</f>
-        <v>0.8</v>
+        <f t="shared" ref="F11" si="10">C11/(C11+D11)</f>
+        <v>0.80327868852459017</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ref="G11:G12" si="11">C11/(C11+C12)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G11" si="11">C11/(C11+C12)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3352,7 +3352,7 @@
       <c r="B12" s="2"/>
       <c r="C12" s="1">
         <f>64-C11</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1">
         <f>56-D11</f>
@@ -3366,21 +3366,21 @@
       <c r="A13" s="2"/>
       <c r="B13" s="3">
         <f>AVERAGE(B3:B12)</f>
-        <v>0.76333333333333331</v>
+        <v>0.76666666666666661</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2">
         <f>AVERAGE(E3:E12)</f>
-        <v>3.8328199999999993E-2</v>
+        <v>3.4289200000000006E-2</v>
       </c>
       <c r="F13" s="3">
         <f>AVERAGE(F3:F12)</f>
-        <v>0.79871910408928959</v>
+        <v>0.79607507461750127</v>
       </c>
       <c r="G13" s="3">
         <f>AVERAGE(G3:G12)</f>
-        <v>0.74375000000000002</v>
+        <v>0.75624999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3424,24 +3424,24 @@
       </c>
       <c r="B19" s="3">
         <f>(C19+D20)/(D20+D19+C19+C20)</f>
-        <v>0.75</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C19" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E19" s="2">
-        <v>0.14422099999999999</v>
+        <v>0.22825999999999999</v>
       </c>
       <c r="F19" s="3">
         <f>C19/(C19+D19)</f>
-        <v>0.77419354838709675</v>
+        <v>0.80327868852459017</v>
       </c>
       <c r="G19" s="3">
         <f>C19/(C19+C20)</f>
-        <v>0.75</v>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,11 +3449,11 @@
       <c r="B20" s="2"/>
       <c r="C20" s="1">
         <f>64-C19</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1">
         <f>56-D19</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -3465,23 +3465,23 @@
       </c>
       <c r="B21" s="3">
         <f t="shared" ref="B21" si="12">(C21+D22)/(D22+D21+C21+C22)</f>
-        <v>0.78333333333333333</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C21" s="1">
         <v>50</v>
       </c>
       <c r="D21" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2">
-        <v>0.17192499999999999</v>
+        <v>0.220579</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:F28" si="13">C21/(C21+D21)</f>
-        <v>0.80645161290322576</v>
+        <f t="shared" ref="F21" si="13">C21/(C21+D21)</f>
+        <v>0.78125</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" ref="G21:G28" si="14">C21/(C21+C22)</f>
+        <f t="shared" ref="G21" si="14">C21/(C21+C22)</f>
         <v>0.78125</v>
       </c>
     </row>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="D22" s="1">
         <f>56-D21</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -3506,24 +3506,24 @@
       </c>
       <c r="B23" s="3">
         <f t="shared" ref="B23" si="15">(C23+D24)/(D24+D23+C23+C24)</f>
-        <v>0.7583333333333333</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="C23" s="1">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="2">
-        <v>0.20243700000000001</v>
+        <v>0.30437700000000001</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ref="F23:F28" si="16">C23/(C23+D23)</f>
-        <v>0.77777777777777779</v>
+        <f t="shared" ref="F23" si="16">C23/(C23+D23)</f>
+        <v>0.796875</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ref="G23:G28" si="17">C23/(C23+C24)</f>
-        <v>0.765625</v>
+        <f t="shared" ref="G23" si="17">C23/(C23+C24)</f>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -3531,11 +3531,11 @@
       <c r="B24" s="2"/>
       <c r="C24" s="1">
         <f>64-C23</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1">
         <f>56-D23</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -3547,24 +3547,24 @@
       </c>
       <c r="B25" s="3">
         <f t="shared" ref="B25" si="18">(C25+D26)/(D26+D25+C25+C26)</f>
-        <v>0.7416666666666667</v>
+        <v>0.7583333333333333</v>
       </c>
       <c r="C25" s="1">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D25" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2">
-        <v>0.173483</v>
+        <v>0.17546999999999999</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" ref="F25:F28" si="19">C25/(C25+D25)</f>
-        <v>0.76190476190476186</v>
+        <f t="shared" ref="F25" si="19">C25/(C25+D25)</f>
+        <v>0.76119402985074625</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G28" si="20">C25/(C25+C26)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G25" si="20">C25/(C25+C26)</f>
+        <v>0.796875</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3572,11 +3572,11 @@
       <c r="B26" s="2"/>
       <c r="C26" s="1">
         <f>64-C25</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D26" s="1">
         <f>56-D25</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -3588,23 +3588,23 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" ref="B27" si="21">(C27+D28)/(D28+D27+C27+C28)</f>
-        <v>0.73333333333333328</v>
+        <v>0.75</v>
       </c>
       <c r="C27" s="1">
         <v>47</v>
       </c>
       <c r="D27" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E27" s="2">
-        <v>0.17216100000000001</v>
+        <v>0.21737600000000001</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" ref="F27:F28" si="22">C27/(C27+D27)</f>
-        <v>0.75806451612903225</v>
+        <f t="shared" ref="F27" si="22">C27/(C27+D27)</f>
+        <v>0.78333333333333333</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" ref="G27:G28" si="23">C27/(C27+C28)</f>
+        <f t="shared" ref="G27" si="23">C27/(C27+C28)</f>
         <v>0.734375</v>
       </c>
     </row>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="D28" s="1">
         <f>56-D27</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -3627,21 +3627,21 @@
       <c r="A29" s="2"/>
       <c r="B29" s="3">
         <f>AVERAGE(B19:B28)</f>
-        <v>0.7533333333333333</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="2">
         <f>AVERAGE(E19:E28)</f>
-        <v>0.17284540000000001</v>
+        <v>0.22921240000000004</v>
       </c>
       <c r="F29" s="3">
         <f>AVERAGE(F19:F28)</f>
-        <v>0.77567844342037895</v>
+        <v>0.78518621034173397</v>
       </c>
       <c r="G29" s="3">
         <f>AVERAGE(G19:G28)</f>
-        <v>0.75624999999999998</v>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3685,24 +3685,24 @@
       </c>
       <c r="B35" s="3">
         <f>(C35+D36)/(D36+D35+C35+C36)</f>
-        <v>0.7583333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="C35" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="1">
         <v>13</v>
       </c>
       <c r="E35" s="2">
-        <v>0.33715899999999999</v>
+        <v>0.31150699999999998</v>
       </c>
       <c r="F35" s="3">
         <f>C35/(C35+D35)</f>
-        <v>0.78688524590163933</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="G35" s="3">
         <f>C35/(C35+C36)</f>
-        <v>0.75</v>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3710,7 +3710,7 @@
       <c r="B36" s="2"/>
       <c r="C36" s="1">
         <f>64-C35</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D36" s="1">
         <f>56-D35</f>
@@ -3726,24 +3726,24 @@
       </c>
       <c r="B37" s="3">
         <f t="shared" ref="B37" si="24">(C37+D38)/(D38+D37+C37+C38)</f>
-        <v>0.7583333333333333</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C37" s="1">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D37" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E37" s="2">
-        <v>0.331347</v>
+        <v>0.31911600000000001</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:F44" si="25">C37/(C37+D37)</f>
-        <v>0.79661016949152541</v>
+        <f t="shared" ref="F37" si="25">C37/(C37+D37)</f>
+        <v>0.78125</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" ref="G37:G44" si="26">C37/(C37+C38)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G37" si="26">C37/(C37+C38)</f>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3751,11 +3751,11 @@
       <c r="B38" s="2"/>
       <c r="C38" s="1">
         <f>64-C37</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D38" s="1">
         <f>56-D37</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -3776,14 +3776,14 @@
         <v>13</v>
       </c>
       <c r="E39" s="2">
-        <v>0.366784</v>
+        <v>0.37185200000000002</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ref="F39:F44" si="28">C39/(C39+D39)</f>
+        <f t="shared" ref="F39" si="28">C39/(C39+D39)</f>
         <v>0.78333333333333333</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" ref="G39:G44" si="29">C39/(C39+C40)</f>
+        <f t="shared" ref="G39" si="29">C39/(C39+C40)</f>
         <v>0.734375</v>
       </c>
     </row>
@@ -3808,24 +3808,24 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" ref="B41" si="30">(C41+D42)/(D42+D41+C41+C42)</f>
-        <v>0.75</v>
+        <v>0.76666666666666672</v>
       </c>
       <c r="C41" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D41" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E41" s="2">
-        <v>0.33833800000000003</v>
+        <v>0.31051600000000001</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ref="F41:F44" si="31">C41/(C41+D41)</f>
-        <v>0.77419354838709675</v>
+        <f t="shared" ref="F41" si="31">C41/(C41+D41)</f>
+        <v>0.79032258064516125</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" ref="G41:G44" si="32">C41/(C41+C42)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G41" si="32">C41/(C41+C42)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3833,11 +3833,11 @@
       <c r="B42" s="2"/>
       <c r="C42" s="1">
         <f>64-C41</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="1">
         <f>56-D41</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -3858,14 +3858,14 @@
         <v>13</v>
       </c>
       <c r="E43" s="2">
-        <v>0.37041600000000002</v>
+        <v>0.33329500000000001</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ref="F43:F44" si="34">C43/(C43+D43)</f>
+        <f t="shared" ref="F43" si="34">C43/(C43+D43)</f>
         <v>0.78688524590163933</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" ref="G43:G44" si="35">C43/(C43+C44)</f>
+        <f t="shared" ref="G43" si="35">C43/(C43+C44)</f>
         <v>0.75</v>
       </c>
     </row>
@@ -3888,21 +3888,21 @@
       <c r="A45" s="2"/>
       <c r="B45" s="3">
         <f>AVERAGE(B35:B44)</f>
-        <v>0.755</v>
+        <v>0.7583333333333333</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="2">
         <f>AVERAGE(E35:E44)</f>
-        <v>0.34880880000000003</v>
+        <v>0.32925719999999997</v>
       </c>
       <c r="F45" s="3">
         <f>AVERAGE(F35:F44)</f>
-        <v>0.78558150860304676</v>
+        <v>0.78502489864269331</v>
       </c>
       <c r="G45" s="3">
         <f>AVERAGE(G35:G44)</f>
-        <v>0.74375000000000002</v>
+        <v>0.75312500000000004</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3916,67 +3916,31 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
@@ -3984,31 +3948,67 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4018,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4059,24 +4059,24 @@
       </c>
       <c r="B3" s="3">
         <f>(C3+D4)/(D4+D3+C3+C4)</f>
-        <v>0.73333333333333328</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="C3" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2">
-        <v>4.7731999999999997E-2</v>
+        <v>3.4556999999999997E-2</v>
       </c>
       <c r="F3" s="3">
         <f>C3/(C3+D3)</f>
-        <v>0.76666666666666672</v>
+        <v>0.7384615384615385</v>
       </c>
       <c r="G3" s="3">
         <f>C3/(C3+C4)</f>
-        <v>0.71875</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4084,11 +4084,11 @@
       <c r="B4" s="2"/>
       <c r="C4" s="1">
         <f>64-C3</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <f>56-D3</f>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4100,23 +4100,23 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ref="B5" si="0">(C5+D6)/(D6+D5+C5+C6)</f>
-        <v>0.75</v>
+        <v>0.7416666666666667</v>
       </c>
       <c r="C5" s="1">
         <v>49</v>
       </c>
       <c r="D5" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>3.6389999999999999E-2</v>
+        <v>3.7289999999999997E-2</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F12" si="1">C5/(C5+D5)</f>
-        <v>0.765625</v>
+        <f t="shared" ref="F5" si="1">C5/(C5+D5)</f>
+        <v>0.75384615384615383</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G12" si="2">C5/(C5+C6)</f>
+        <f t="shared" ref="G5" si="2">C5/(C5+C6)</f>
         <v>0.765625</v>
       </c>
     </row>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="D6" s="1">
         <f>56-D5</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -4144,21 +4144,21 @@
         <v>0.76666666666666672</v>
       </c>
       <c r="C7" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2">
-        <v>3.3699E-2</v>
+        <v>3.4787999999999999E-2</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F12" si="4">C7/(C7+D7)</f>
-        <v>0.79032258064516125</v>
+        <f t="shared" ref="F7" si="4">C7/(C7+D7)</f>
+        <v>0.78125</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7:G12" si="5">C7/(C7+C8)</f>
-        <v>0.765625</v>
+        <f t="shared" ref="G7" si="5">C7/(C7+C8)</f>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4166,11 +4166,11 @@
       <c r="B8" s="2"/>
       <c r="C8" s="1">
         <f>64-C7</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1">
         <f>56-D7</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -4182,24 +4182,24 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ref="B9" si="6">(C9+D10)/(D10+D9+C9+C10)</f>
-        <v>0.72499999999999998</v>
+        <v>0.7416666666666667</v>
       </c>
       <c r="C9" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2">
-        <v>3.5379000000000001E-2</v>
+        <v>3.4039E-2</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F12" si="7">C9/(C9+D9)</f>
-        <v>0.74603174603174605</v>
+        <f t="shared" ref="F9" si="7">C9/(C9+D9)</f>
+        <v>0.76190476190476186</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" ref="G9:G12" si="8">C9/(C9+C10)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G9" si="8">C9/(C9+C10)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4207,11 +4207,11 @@
       <c r="B10" s="2"/>
       <c r="C10" s="1">
         <f>64-C9</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
         <f>56-D9</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4223,24 +4223,24 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ref="B11" si="9">(C11+D12)/(D12+D11+C11+C12)</f>
-        <v>0.76666666666666672</v>
+        <v>0.75</v>
       </c>
       <c r="C11" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2">
-        <v>3.6451999999999998E-2</v>
+        <v>3.2532999999999999E-2</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ref="F11:F12" si="10">C11/(C11+D11)</f>
-        <v>0.81034482758620685</v>
+        <f t="shared" ref="F11" si="10">C11/(C11+D11)</f>
+        <v>0.77419354838709675</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ref="G11:G12" si="11">C11/(C11+C12)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G11" si="11">C11/(C11+C12)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4248,11 +4248,11 @@
       <c r="B12" s="2"/>
       <c r="C12" s="1">
         <f>64-C11</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1">
         <f>56-D11</f>
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -4262,21 +4262,21 @@
       <c r="A13" s="2"/>
       <c r="B13" s="3">
         <f>AVERAGE(B3:B12)</f>
-        <v>0.74833333333333329</v>
+        <v>0.745</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2">
         <f>AVERAGE(E3:E12)</f>
-        <v>3.7930399999999996E-2</v>
+        <v>3.4641400000000003E-2</v>
       </c>
       <c r="F13" s="3">
         <f>AVERAGE(F3:F12)</f>
-        <v>0.77579816418595615</v>
+        <v>0.76193120051991026</v>
       </c>
       <c r="G13" s="3">
         <f>AVERAGE(G3:G12)</f>
-        <v>0.74375000000000002</v>
+        <v>0.75937500000000002</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4323,21 +4323,21 @@
         <v>0.71666666666666667</v>
       </c>
       <c r="C19" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2">
-        <v>0.69508599999999998</v>
+        <v>1.0544309999999999</v>
       </c>
       <c r="F19" s="3">
         <f>C19/(C19+D19)</f>
-        <v>0.734375</v>
+        <v>0.74193548387096775</v>
       </c>
       <c r="G19" s="3">
         <f>C19/(C19+C20)</f>
-        <v>0.734375</v>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4345,11 +4345,11 @@
       <c r="B20" s="2"/>
       <c r="C20" s="1">
         <f>64-C19</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1">
         <f>56-D19</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -4361,24 +4361,24 @@
       </c>
       <c r="B21" s="3">
         <f t="shared" ref="B21" si="12">(C21+D22)/(D22+D21+C21+C22)</f>
-        <v>0.7416666666666667</v>
+        <v>0.7583333333333333</v>
       </c>
       <c r="C21" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1">
         <v>14</v>
       </c>
       <c r="E21" s="2">
-        <v>0.55771800000000005</v>
+        <v>0.65324499999999996</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:F28" si="13">C21/(C21+D21)</f>
-        <v>0.77049180327868849</v>
+        <f t="shared" ref="F21" si="13">C21/(C21+D21)</f>
+        <v>0.77777777777777779</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" ref="G21:G28" si="14">C21/(C21+C22)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G21" si="14">C21/(C21+C22)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4386,7 +4386,7 @@
       <c r="B22" s="2"/>
       <c r="C22" s="1">
         <f>64-C21</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1">
         <f>56-D21</f>
@@ -4402,24 +4402,24 @@
       </c>
       <c r="B23" s="3">
         <f t="shared" ref="B23" si="15">(C23+D24)/(D24+D23+C23+C24)</f>
-        <v>0.72499999999999998</v>
+        <v>0.7583333333333333</v>
       </c>
       <c r="C23" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E23" s="2">
-        <v>0.99537200000000003</v>
+        <v>0.82169700000000001</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ref="F23:F28" si="16">C23/(C23+D23)</f>
-        <v>0.74603174603174605</v>
+        <f t="shared" ref="F23" si="16">C23/(C23+D23)</f>
+        <v>0.77777777777777779</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ref="G23:G28" si="17">C23/(C23+C24)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G23" si="17">C23/(C23+C24)</f>
+        <v>0.765625</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -4427,11 +4427,11 @@
       <c r="B24" s="2"/>
       <c r="C24" s="1">
         <f>64-C23</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1">
         <f>56-D23</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -4443,24 +4443,24 @@
       </c>
       <c r="B25" s="3">
         <f t="shared" ref="B25" si="18">(C25+D26)/(D26+D25+C25+C26)</f>
-        <v>0.7</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="C25" s="1">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E25" s="2">
-        <v>0.68391500000000005</v>
+        <v>0.70254799999999995</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" ref="F25:F28" si="19">C25/(C25+D25)</f>
-        <v>0.74137931034482762</v>
+        <f t="shared" ref="F25" si="19">C25/(C25+D25)</f>
+        <v>0.734375</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G28" si="20">C25/(C25+C26)</f>
-        <v>0.671875</v>
+        <f t="shared" ref="G25" si="20">C25/(C25+C26)</f>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4468,11 +4468,11 @@
       <c r="B26" s="2"/>
       <c r="C26" s="1">
         <f>64-C25</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1">
         <f>56-D25</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -4484,24 +4484,24 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" ref="B27" si="21">(C27+D28)/(D28+D27+C27+C28)</f>
-        <v>0.71666666666666667</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="C27" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E27" s="2">
-        <v>0.90190999999999999</v>
+        <v>0.82996300000000001</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" ref="F27:F28" si="22">C27/(C27+D27)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="F27" si="22">C27/(C27+D27)</f>
+        <v>0.76666666666666672</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" ref="G27:G28" si="23">C27/(C27+C28)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G27" si="23">C27/(C27+C28)</f>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4509,11 +4509,11 @@
       <c r="B28" s="2"/>
       <c r="C28" s="1">
         <f>64-C27</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1">
         <f>56-D27</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -4523,21 +4523,21 @@
       <c r="A29" s="2"/>
       <c r="B29" s="3">
         <f>AVERAGE(B19:B28)</f>
-        <v>0.72000000000000008</v>
+        <v>0.73666666666666669</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="2">
         <f>AVERAGE(E19:E28)</f>
-        <v>0.76680019999999993</v>
+        <v>0.81237680000000001</v>
       </c>
       <c r="F29" s="3">
         <f>AVERAGE(F19:F28)</f>
-        <v>0.74533057193105245</v>
+        <v>0.75970654121863801</v>
       </c>
       <c r="G29" s="3">
         <f>AVERAGE(G19:G28)</f>
-        <v>0.72187500000000004</v>
+        <v>0.74062499999999998</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -4590,7 +4590,7 @@
         <v>16</v>
       </c>
       <c r="E35" s="2">
-        <v>0.606155</v>
+        <v>0.63653300000000002</v>
       </c>
       <c r="F35" s="3">
         <f>C35/(C35+D35)</f>
@@ -4622,24 +4622,24 @@
       </c>
       <c r="B37" s="3">
         <f t="shared" ref="B37" si="24">(C37+D38)/(D38+D37+C37+C38)</f>
-        <v>0.7416666666666667</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="C37" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="1">
         <v>14</v>
       </c>
       <c r="E37" s="2">
-        <v>0.50526400000000005</v>
+        <v>0.547126</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:F44" si="25">C37/(C37+D37)</f>
-        <v>0.77049180327868849</v>
+        <f t="shared" ref="F37" si="25">C37/(C37+D37)</f>
+        <v>0.76666666666666672</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" ref="G37:G44" si="26">C37/(C37+C38)</f>
-        <v>0.734375</v>
+        <f t="shared" ref="G37" si="26">C37/(C37+C38)</f>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -4647,7 +4647,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="1">
         <f>64-C37</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D38" s="1">
         <f>56-D37</f>
@@ -4663,24 +4663,24 @@
       </c>
       <c r="B39" s="3">
         <f t="shared" ref="B39" si="27">(C39+D40)/(D40+D39+C39+C40)</f>
-        <v>0.72499999999999998</v>
+        <v>0.7416666666666667</v>
       </c>
       <c r="C39" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" s="2">
-        <v>0.55088300000000001</v>
+        <v>0.55562999999999996</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ref="F39:F44" si="28">C39/(C39+D39)</f>
-        <v>0.75409836065573765</v>
+        <f t="shared" ref="F39" si="28">C39/(C39+D39)</f>
+        <v>0.77049180327868849</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" ref="G39:G44" si="29">C39/(C39+C40)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G39" si="29">C39/(C39+C40)</f>
+        <v>0.734375</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4688,11 +4688,11 @@
       <c r="B40" s="2"/>
       <c r="C40" s="1">
         <f>64-C39</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="1">
         <f>56-D39</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -4704,24 +4704,24 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" ref="B41" si="30">(C41+D42)/(D42+D41+C41+C42)</f>
-        <v>0.72499999999999998</v>
+        <v>0.7</v>
       </c>
       <c r="C41" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D41" s="1">
         <v>15</v>
       </c>
       <c r="E41" s="2">
-        <v>0.61264700000000005</v>
+        <v>0.55305700000000002</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ref="F41:F44" si="31">C41/(C41+D41)</f>
-        <v>0.75409836065573765</v>
+        <f t="shared" ref="F41" si="31">C41/(C41+D41)</f>
+        <v>0.74137931034482762</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" ref="G41:G44" si="32">C41/(C41+C42)</f>
-        <v>0.71875</v>
+        <f t="shared" ref="G41" si="32">C41/(C41+C42)</f>
+        <v>0.671875</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -4729,7 +4729,7 @@
       <c r="B42" s="2"/>
       <c r="C42" s="1">
         <f>64-C41</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D42" s="1">
         <f>56-D41</f>
@@ -4754,14 +4754,14 @@
         <v>14</v>
       </c>
       <c r="E43" s="2">
-        <v>0.501911</v>
+        <v>0.53713699999999998</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ref="F43:F44" si="34">C43/(C43+D43)</f>
+        <f t="shared" ref="F43" si="34">C43/(C43+D43)</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" ref="G43:G44" si="35">C43/(C43+C44)</f>
+        <f t="shared" ref="G43" si="35">C43/(C43+C44)</f>
         <v>0.6875</v>
       </c>
     </row>
@@ -4784,21 +4784,21 @@
       <c r="A45" s="2"/>
       <c r="B45" s="3">
         <f>AVERAGE(B35:B44)</f>
-        <v>0.72166666666666668</v>
+        <v>0.71833333333333338</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="2">
         <f>AVERAGE(E35:E44)</f>
-        <v>0.55537199999999998</v>
+        <v>0.56589659999999997</v>
       </c>
       <c r="F45" s="3">
         <f>AVERAGE(F35:F44)</f>
-        <v>0.75412850951573385</v>
+        <v>0.75409836065573776</v>
       </c>
       <c r="G45" s="3">
         <f>AVERAGE(G35:G44)</f>
-        <v>0.70937499999999998</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -4812,62 +4812,34 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="C18:D18"/>
@@ -4876,35 +4848,63 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>